<commit_message>
reading from excel and quiz selector and routes
</commit_message>
<xml_diff>
--- a/example/data.xlsx
+++ b/example/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\samsat-quiz-app\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C74A24C-6944-4C9E-A11B-7465E76B4189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B820EF-1D75-463A-9141-F6AA823F30C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3015" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24300" yWindow="1785" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
     <sheet name="Quiz1" sheetId="2" r:id="rId2"/>
+    <sheet name="Quiz2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -391,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,23 +549,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6E16CF-BF9E-43CD-82E7-EA9567C3AE6F}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C1C905-5E3D-4F98-83EA-1A1AC8B7A352}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>